<commit_message>
LTHDT-LT-Tuan03. Hoan thanh Bai 2 (2/2).
</commit_message>
<xml_diff>
--- a/LTHDT_LT_Tuan03_PhamThanhTung/demo/LopHP_LT_Tuan03_testcase.xlsx
+++ b/LTHDT_LT_Tuan03_PhamThanhTung/demo/LopHP_LT_Tuan03_testcase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\@@@LTHDT_HocKyI_20232024\7_BaitapTuan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\workspaces\uni_c2023_2024_s1_java_oop_exercises\LTHDT_LT_Tuan03_PhamThanhTung\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD898D5-732D-42CB-A639-7D7A7B5E2E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D4005F-0E36-4E6F-8796-22E4015F6B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14310" yWindow="0" windowWidth="14580" windowHeight="17370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
   <si>
     <t>Passed</t>
   </si>
@@ -51,36 +62,12 @@
     <t>Kết quả mong muốn</t>
   </si>
   <si>
-    <t>Họ tên:</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mã số sinh viên: </t>
   </si>
   <si>
-    <t>foo(1, 2, 1, 2)</t>
-  </si>
-  <si>
-    <t>java.lang.ArithmeticException: / by zero</t>
-  </si>
-  <si>
-    <t>foo(1, 1, 1, 1)</t>
-  </si>
-  <si>
     <t>Báo cáo kết quả kiểm thử</t>
   </si>
   <si>
-    <t>float foo(int a, int b, int c, int d) {
-      float e;
-      if (a==0)
-           return 0;
-      int x = 0;
-      if ((a==b) || (c==d))
-           x = 1;
-      e = 1/x;
-   return e;
- }</t>
-  </si>
-  <si>
     <t>Passed:</t>
   </si>
   <si>
@@ -93,38 +80,204 @@
     <t>Lớp test</t>
   </si>
   <si>
-    <t>MyClass</t>
-  </si>
-  <si>
     <t>STT</t>
   </si>
   <si>
-    <t>Lớp:</t>
-  </si>
-  <si>
     <t>Dữ liệu đầu vào</t>
   </si>
   <si>
-    <t>a=0, b=0, c=0, d=0</t>
-  </si>
-  <si>
-    <t>Test cho trường hợp a=0, kết hợp test cho a=b, c=d</t>
-  </si>
-  <si>
-    <t>Test cho trường hợp a&lt;&gt;0, kết hợp test cho a=b, c=d</t>
-  </si>
-  <si>
-    <t>Test cho trường hợp a&lt;&gt;0, kết hợp test cho a&lt;&gt;b, c&lt;&gt;d</t>
-  </si>
-  <si>
-    <t>testFoo</t>
+    <t>oldQuantity=6638, newQuantity=7298</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>Họ tên: Phạm Thanh Tùng</t>
+  </si>
+  <si>
+    <t>Lớp: Lập trình hướng đối tượng</t>
+  </si>
+  <si>
+    <t>public static double totalAmount(int oldQuantity, int newQuantity){
+        int consumedQuantity = newQuantity - oldQuantity;
+        if (consumedQuantity &lt; 0) {
+            throw new RuntimeException("Không thể thành tiền hoá đơn vì hiệu số âm.");
+        }
+        int levelQuantity = 0;
+        double amount = 0.0;
+        for (int i = 0; i &lt; 6; i++) {
+            switch (i) {
+                case 0: // 0-50: tiền đối đa = 86400
+                    if (consumedQuantity &gt; 50) {
+                        levelQuantity = 50;
+                        consumedQuantity -= 50;
+                    } else {
+                        levelQuantity = consumedQuantity;
+                        consumedQuantity = 0;
+                    }
+                    amount += (double) levelQuantity * 1728;
+                    break;
+                case 1: // 51-100: tiền đối đa = 89300
+                    if (consumedQuantity &gt; 50) {
+                        levelQuantity = 50;
+                        consumedQuantity -= 50;
+                    } else {
+                        levelQuantity = consumedQuantity;
+                        consumedQuantity = 0;
+                    }
+                    amount += (double) levelQuantity * 1786;
+                    break;
+                case 2: // 101-200: tiền đối đa = 207400
+                    if (consumedQuantity &gt; 100) {
+                        levelQuantity = 100;
+                        consumedQuantity -= 100;
+                    } else {
+                        levelQuantity = consumedQuantity;
+                        consumedQuantity = 0;
+                    }
+                    amount += (double) levelQuantity * 2074;
+                    break;
+                case 3: // 201-300: tiền đối đa = 261200
+                    if (consumedQuantity &gt; 100) {
+                        levelQuantity = 100;
+                        consumedQuantity -= 100;
+                    } else {
+                        levelQuantity = consumedQuantity;
+                        consumedQuantity = 0;
+                    }
+                    amount += (double) levelQuantity * 2612;
+                    break;
+                case 4: // 301-400: tiền đối đa = 291900
+                    if (consumedQuantity &gt; 100) {
+                        levelQuantity = 100;
+                        consumedQuantity -= 100;
+                    } else {
+                        levelQuantity = consumedQuantity;
+                        consumedQuantity = 0;
+                    }
+                    amount += (double) levelQuantity * 2919;
+                    break;
+                case 5: // 401+
+                    levelQuantity = consumedQuantity;
+                    consumedQuantity = 0;
+                    amount += (double) levelQuantity * 3015;
+                    break;
+                default: break;
+            }
+        }
+        double VAT_RATE = 0.1;
+        double totalVATAmount = amount * VAT_RATE;
+        return Math.ceil(amount + totalVATAmount);
+}</t>
+  </si>
+  <si>
+    <t>public static int getTienDien(int chiSoCu, int chiSoMoi){
+        final double THUE = 0.1; // Thuế VAT
+        int soKWh = chiSoMoi - chiSoCu; // Số kWh tiêu thụ
+        int tienDien = getSoKWh(soKWh, 400, Integer.MAX_VALUE) * 3015
+                + getSoKWh(soKWh, 300, 400) * 2919
+                + getSoKWh(soKWh, 200, 300) * 2612
+                + getSoKWh(soKWh, 100, 200) * 2074
+                + getSoKWh(soKWh, 50, 100) * 1786
+                + getSoKWh(soKWh, 0, 50) * 1728;
+        return tienDien + (int)Math.ceil(tienDien * THUE);
+    }
+public static int getSoKWh(int soKWh, int soDau, int soCuoi){
+        if(soKWh &lt; soDau)
+            return 0;
+        if(soKWh &lt;= soCuoi)
+            return soKWh - soDau;
+        return soCuoi - soDau;
+}</t>
+  </si>
+  <si>
+    <t>ElectricityConsumptionCalculatorTest</t>
+  </si>
+  <si>
+    <t>oldQuantity=5689, newQuantity=6638</t>
+  </si>
+  <si>
+    <t>oldQuantity=5640, newQuantity=5689</t>
+  </si>
+  <si>
+    <t>oldQuantity=5467, newQuantity=5640</t>
+  </si>
+  <si>
+    <t>oldQuantity=5467, newQuantity=5467</t>
+  </si>
+  <si>
+    <t>oldQuantity=5417, newQuantity=5467</t>
+  </si>
+  <si>
+    <t>oldQuantity=5000, newQuantity=5087</t>
+  </si>
+  <si>
+    <t>oldQuantity=5000, newQuantity=5245</t>
+  </si>
+  <si>
+    <t>oldQuantity=5000, newQuantity=5367</t>
+  </si>
+  <si>
+    <t>oldQuantity=5000, newQuantity=4990</t>
+  </si>
+  <si>
+    <t>java.lang.RuntimeException: Không thể thành tiền hoá đơn vì hiệu số âm.</t>
+  </si>
+  <si>
+    <t>Test cho trường hợp lượng điện tiêu thụ là 660</t>
+  </si>
+  <si>
+    <t>Test cho trường hợp lượng điện tiêu thụ là 949</t>
+  </si>
+  <si>
+    <t>Test cho trường hợp lượng điện tiêu thụ là 49</t>
+  </si>
+  <si>
+    <t>Test cho trường hợp lượng điện tiêu thụ là 173</t>
+  </si>
+  <si>
+    <t>Test cho trường hợp lượng điện tiêu thụ là 0</t>
+  </si>
+  <si>
+    <t>Test cho trường hợp lượng điện tiêu thụ là 50</t>
+  </si>
+  <si>
+    <t>Test cho trường hợp lượng điện tiêu thụ là số âm.
+Ví dụ -10</t>
+  </si>
+  <si>
+    <t>Test cho trường hợp lượng điện tiêu thụ là 100</t>
+  </si>
+  <si>
+    <t>Test cho trường hợp lượng điện tiêu thụ là 200</t>
+  </si>
+  <si>
+    <t>Test cho trường hợp lượng điện tiêu thụ là 300</t>
+  </si>
+  <si>
+    <t>Test cho trường hợp lượng điện tiêu thụ là 400</t>
+  </si>
+  <si>
+    <t>oldQuantity=5000, newQuantity=5400</t>
+  </si>
+  <si>
+    <t>oldQuantity=5000, newQuantity=5300</t>
+  </si>
+  <si>
+    <t>oldQuantity=5000, newQuantity=5200</t>
+  </si>
+  <si>
+    <t>oldQuantity=5000, newQuantity=5100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +316,23 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -252,7 +422,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -271,12 +441,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -293,12 +459,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -307,6 +467,39 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -623,99 +816,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="46.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="51" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.6328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.1796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.26953125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3">
+        <f>COUNTIF(I6:I26,"passed")</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="3">
+        <f>COUNTIF(I6:I26,"failed")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="3">
+        <f>COUNTA(I6:I26)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="3">
-        <f>COUNTIF(I6:I8,"passed")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="3">
-        <f>COUNTIF(I6:I8,"failed")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="3">
-        <f>COUNTA(I6:I8)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>4</v>
@@ -727,7 +920,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>7</v>
@@ -739,157 +932,535 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>1</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>27</v>
+      <c r="B6" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0</v>
+        <v>1892110</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1892110</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>2</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="19"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="15"/>
       <c r="E7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>12</v>
+        <v>35</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="G7" s="6">
-        <v>1</v>
-      </c>
-      <c r="H7" s="7">
-        <v>1</v>
+        <v>2850579</v>
+      </c>
+      <c r="H7" s="6">
+        <v>2850579</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>3</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="20"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="6">
+        <v>93140</v>
+      </c>
+      <c r="H8" s="6">
+        <v>93140</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>4</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G9" s="6">
+        <v>359813</v>
+      </c>
+      <c r="H9" s="6">
+        <v>359813</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>5</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>6</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="6">
+        <v>95040</v>
+      </c>
+      <c r="H11" s="6">
+        <v>95040</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>7</v>
+      </c>
+      <c r="B12" s="22"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="6">
+        <v>193270</v>
+      </c>
+      <c r="H12" s="6">
+        <v>193270</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>8</v>
+      </c>
+      <c r="B13" s="22"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="6">
+        <v>421410</v>
+      </c>
+      <c r="H13" s="6">
+        <v>421410</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>9</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="20">
+        <v>708730</v>
+      </c>
+      <c r="H14" s="20">
+        <v>708730</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
         <v>10</v>
       </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
-      <c r="H8" s="7" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="20">
+        <v>1029820</v>
+      </c>
+      <c r="H15" s="20">
+        <v>1029820</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
         <v>11</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="20">
+        <v>0</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>12</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1892110</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1892110</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>13</v>
+      </c>
+      <c r="B18" s="22"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="6">
+        <v>2850579</v>
+      </c>
+      <c r="H18" s="6">
+        <v>2850579</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>14</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="6">
+        <v>93140</v>
+      </c>
+      <c r="H19" s="6">
+        <v>93140</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>15</v>
+      </c>
+      <c r="B20" s="22"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="6">
+        <v>359813</v>
+      </c>
+      <c r="H20" s="6">
+        <v>359813</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>16</v>
+      </c>
+      <c r="B21" s="22"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>17</v>
+      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="6">
+        <v>95040</v>
+      </c>
+      <c r="H22" s="6">
+        <v>95040</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>18</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="6">
+        <v>193270</v>
+      </c>
+      <c r="H23" s="6">
+        <v>193270</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>19</v>
+      </c>
+      <c r="B24" s="22"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="6">
+        <v>421410</v>
+      </c>
+      <c r="H24" s="6">
+        <v>421410</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>20</v>
+      </c>
+      <c r="B25" s="22"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="20">
+        <v>708730</v>
+      </c>
+      <c r="H25" s="20">
+        <v>708730</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>21</v>
+      </c>
+      <c r="B26" s="22"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="20">
+        <v>1029820</v>
+      </c>
+      <c r="H26" s="20">
+        <v>1029820</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="46" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>22</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="20">
+        <v>0</v>
+      </c>
+      <c r="H27" s="20">
+        <v>0</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B6:B8"/>
+  <mergeCells count="9">
+    <mergeCell ref="D6:D16"/>
+    <mergeCell ref="C17:C27"/>
+    <mergeCell ref="D17:D27"/>
+    <mergeCell ref="B6:B27"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A4:G4"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C6:C16"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>